<commit_message>
Added some test examples to the xlsx file
</commit_message>
<xml_diff>
--- a/testSet.xlsx
+++ b/testSet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f8defdd50762089b/UNI/OD-UNI_Sommersemester2023/BachelorThesis/automaticHintGeneration/automaticHintGeneration/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexOKRE\BachelorThesis\optimizationOfHintGeneration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="11_AD4DB114E441178AC67DF48C0E97C61C693EDF1A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFE58893-8095-4155-A55A-B4695DE8C234}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2703B41-1F99-4042-8A14-8C6EA018B333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Question</t>
   </si>
@@ -55,6 +55,24 @@
   </si>
   <si>
     <t>In which year was the Euro as payment method introduced?</t>
+  </si>
+  <si>
+    <t>Who is the president of the USA?</t>
+  </si>
+  <si>
+    <t>Joe Biden</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>When did Miachel Schumacher win his first F1 World Drivers Title?</t>
+  </si>
+  <si>
+    <t>Max Verstappen</t>
+  </si>
+  <si>
+    <t>Who was the F1 World Champion in 2022?</t>
   </si>
 </sst>
 </file>
@@ -107,10 +125,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -376,15 +390,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="66.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -431,6 +446,39 @@
         <v>8</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>1994</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modified/extended testSet.xlsx for new tests.
</commit_message>
<xml_diff>
--- a/testSet.xlsx
+++ b/testSet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexOKRE\BachelorThesis\optimizationOfHintGeneration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexOKRE\BachelorThesis\TestBranch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2703B41-1F99-4042-8A14-8C6EA018B333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE19DB4A-540E-424B-B05F-12EC528972A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>Question</t>
   </si>
@@ -36,12 +36,6 @@
     <t>Category</t>
   </si>
   <si>
-    <t>General Franco became leader of which country in 1939 after a Civil War?</t>
-  </si>
-  <si>
-    <t>Spain</t>
-  </si>
-  <si>
     <t>Location</t>
   </si>
   <si>
@@ -57,12 +51,6 @@
     <t>In which year was the Euro as payment method introduced?</t>
   </si>
   <si>
-    <t>Who is the president of the USA?</t>
-  </si>
-  <si>
-    <t>Joe Biden</t>
-  </si>
-  <si>
     <t>Person</t>
   </si>
   <si>
@@ -73,6 +61,30 @@
   </si>
   <si>
     <t>Who was the F1 World Champion in 2022?</t>
+  </si>
+  <si>
+    <t>When did Miachel Schumacher win his 2nd F1 World Drivers Title?</t>
+  </si>
+  <si>
+    <t>When did Miachel Schumacher win his 3rd F1 World Drivers Title?</t>
+  </si>
+  <si>
+    <t>When did Miachel Schumacher win his 4th F1 World Drivers Title?</t>
+  </si>
+  <si>
+    <t>When did Miachel Schumacher win his 5th F1 World Drivers Title?</t>
+  </si>
+  <si>
+    <t>When did Miachel Schumacher win his 6th F1 World Drivers Title?</t>
+  </si>
+  <si>
+    <t>When did Miachel Schumacher win his 7th F1 World Drivers Title?</t>
+  </si>
+  <si>
+    <t>When has Chelsea last won the Champions League?</t>
+  </si>
+  <si>
+    <t>When was the World Cup last won by Italy?</t>
   </si>
 </sst>
 </file>
@@ -390,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,24 +427,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -440,43 +452,109 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>1999</v>
+        <v>1994</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5">
-        <v>1994</v>
+        <v>1995</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>1999</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>2000</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>2001</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
+      <c r="B9">
+        <v>2002</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>2003</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>2004</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12">
+        <v>2006</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>2021</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>